<commit_message>
display limit set to 10
</commit_message>
<xml_diff>
--- a/view/site/new.xlsx
+++ b/view/site/new.xlsx
@@ -402,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E15" sqref="E15"/>
@@ -686,6 +686,312 @@
         <v>7.4</v>
       </c>
       <c r="E16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E34" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set responsive to profile
</commit_message>
<xml_diff>
--- a/view/site/new.xlsx
+++ b/view/site/new.xlsx
@@ -402,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E15" sqref="E15"/>
@@ -3848,6 +3848,924 @@
         <v>7.4</v>
       </c>
       <c r="E202" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B203" s="1">
+        <v>8</v>
+      </c>
+      <c r="C203" s="1">
+        <v>5</v>
+      </c>
+      <c r="D203" s="1">
+        <v>8</v>
+      </c>
+      <c r="E203" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B204" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C204" s="1">
+        <v>5</v>
+      </c>
+      <c r="D204" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E204" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B205" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C205" s="1">
+        <v>5</v>
+      </c>
+      <c r="D205" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E205" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B206" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C206" s="1">
+        <v>5</v>
+      </c>
+      <c r="D206" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E206" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B207" s="1">
+        <v>8</v>
+      </c>
+      <c r="C207" s="1">
+        <v>5</v>
+      </c>
+      <c r="D207" s="1">
+        <v>8</v>
+      </c>
+      <c r="E207" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B208" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C208" s="1">
+        <v>5</v>
+      </c>
+      <c r="D208" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E208" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209" s="1">
+        <v>8</v>
+      </c>
+      <c r="C209" s="1">
+        <v>5</v>
+      </c>
+      <c r="D209" s="1">
+        <v>8</v>
+      </c>
+      <c r="E209" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B210" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C210" s="1">
+        <v>5</v>
+      </c>
+      <c r="D210" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E210" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B211" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C211" s="1">
+        <v>5</v>
+      </c>
+      <c r="D211" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E211" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B212" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C212" s="1">
+        <v>5</v>
+      </c>
+      <c r="D212" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E212" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B213" s="1">
+        <v>8</v>
+      </c>
+      <c r="C213" s="1">
+        <v>5</v>
+      </c>
+      <c r="D213" s="1">
+        <v>8</v>
+      </c>
+      <c r="E213" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B214" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C214" s="1">
+        <v>5</v>
+      </c>
+      <c r="D214" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E214" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B215" s="1">
+        <v>8</v>
+      </c>
+      <c r="C215" s="1">
+        <v>5</v>
+      </c>
+      <c r="D215" s="1">
+        <v>8</v>
+      </c>
+      <c r="E215" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B216" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C216" s="1">
+        <v>5</v>
+      </c>
+      <c r="D216" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E216" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B217" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C217" s="1">
+        <v>5</v>
+      </c>
+      <c r="D217" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E217" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B218" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C218" s="1">
+        <v>5</v>
+      </c>
+      <c r="D218" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E218" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B219" s="1">
+        <v>8</v>
+      </c>
+      <c r="C219" s="1">
+        <v>5</v>
+      </c>
+      <c r="D219" s="1">
+        <v>8</v>
+      </c>
+      <c r="E219" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B220" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C220" s="1">
+        <v>5</v>
+      </c>
+      <c r="D220" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E220" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B221" s="1">
+        <v>8</v>
+      </c>
+      <c r="C221" s="1">
+        <v>5</v>
+      </c>
+      <c r="D221" s="1">
+        <v>8</v>
+      </c>
+      <c r="E221" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B222" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C222" s="1">
+        <v>5</v>
+      </c>
+      <c r="D222" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E222" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B223" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C223" s="1">
+        <v>5</v>
+      </c>
+      <c r="D223" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E223" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B224" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C224" s="1">
+        <v>5</v>
+      </c>
+      <c r="D224" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E224" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B225" s="1">
+        <v>8</v>
+      </c>
+      <c r="C225" s="1">
+        <v>5</v>
+      </c>
+      <c r="D225" s="1">
+        <v>8</v>
+      </c>
+      <c r="E225" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B226" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C226" s="1">
+        <v>5</v>
+      </c>
+      <c r="D226" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E226" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B227" s="1">
+        <v>8</v>
+      </c>
+      <c r="C227" s="1">
+        <v>5</v>
+      </c>
+      <c r="D227" s="1">
+        <v>8</v>
+      </c>
+      <c r="E227" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B228" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C228" s="1">
+        <v>5</v>
+      </c>
+      <c r="D228" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E228" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B229" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C229" s="1">
+        <v>5</v>
+      </c>
+      <c r="D229" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E229" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B230" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C230" s="1">
+        <v>5</v>
+      </c>
+      <c r="D230" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E230" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B231" s="1">
+        <v>8</v>
+      </c>
+      <c r="C231" s="1">
+        <v>5</v>
+      </c>
+      <c r="D231" s="1">
+        <v>8</v>
+      </c>
+      <c r="E231" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B232" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C232" s="1">
+        <v>5</v>
+      </c>
+      <c r="D232" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E232" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B233" s="1">
+        <v>8</v>
+      </c>
+      <c r="C233" s="1">
+        <v>5</v>
+      </c>
+      <c r="D233" s="1">
+        <v>8</v>
+      </c>
+      <c r="E233" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B234" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C234" s="1">
+        <v>5</v>
+      </c>
+      <c r="D234" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E234" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B235" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C235" s="1">
+        <v>5</v>
+      </c>
+      <c r="D235" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E235" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B236" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C236" s="1">
+        <v>5</v>
+      </c>
+      <c r="D236" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E236" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B237" s="1">
+        <v>8</v>
+      </c>
+      <c r="C237" s="1">
+        <v>5</v>
+      </c>
+      <c r="D237" s="1">
+        <v>8</v>
+      </c>
+      <c r="E237" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B238" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C238" s="1">
+        <v>5</v>
+      </c>
+      <c r="D238" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E238" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B239" s="1">
+        <v>8</v>
+      </c>
+      <c r="C239" s="1">
+        <v>5</v>
+      </c>
+      <c r="D239" s="1">
+        <v>8</v>
+      </c>
+      <c r="E239" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B240" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C240" s="1">
+        <v>5</v>
+      </c>
+      <c r="D240" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E240" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B241" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C241" s="1">
+        <v>5</v>
+      </c>
+      <c r="D241" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E241" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B242" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C242" s="1">
+        <v>5</v>
+      </c>
+      <c r="D242" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E242" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B243" s="1">
+        <v>8</v>
+      </c>
+      <c r="C243" s="1">
+        <v>5</v>
+      </c>
+      <c r="D243" s="1">
+        <v>8</v>
+      </c>
+      <c r="E243" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B244" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C244" s="1">
+        <v>5</v>
+      </c>
+      <c r="D244" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E244" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B245" s="1">
+        <v>8</v>
+      </c>
+      <c r="C245" s="1">
+        <v>5</v>
+      </c>
+      <c r="D245" s="1">
+        <v>8</v>
+      </c>
+      <c r="E245" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B246" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C246" s="1">
+        <v>5</v>
+      </c>
+      <c r="D246" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E246" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B247" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C247" s="1">
+        <v>5</v>
+      </c>
+      <c r="D247" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E247" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B248" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C248" s="1">
+        <v>5</v>
+      </c>
+      <c r="D248" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E248" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B249" s="1">
+        <v>8</v>
+      </c>
+      <c r="C249" s="1">
+        <v>5</v>
+      </c>
+      <c r="D249" s="1">
+        <v>8</v>
+      </c>
+      <c r="E249" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B250" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C250" s="1">
+        <v>5</v>
+      </c>
+      <c r="D250" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E250" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B251" s="1">
+        <v>8</v>
+      </c>
+      <c r="C251" s="1">
+        <v>5</v>
+      </c>
+      <c r="D251" s="1">
+        <v>8</v>
+      </c>
+      <c r="E251" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B252" s="1">
+        <v>8.3</v>
+      </c>
+      <c r="C252" s="1">
+        <v>5</v>
+      </c>
+      <c r="D252" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="E252" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
+      <c r="A253" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B253" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C253" s="1">
+        <v>5</v>
+      </c>
+      <c r="D253" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="E253" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B254" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C254" s="1">
+        <v>5</v>
+      </c>
+      <c r="D254" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E254" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B255" s="1">
+        <v>8</v>
+      </c>
+      <c r="C255" s="1">
+        <v>5</v>
+      </c>
+      <c r="D255" s="1">
+        <v>8</v>
+      </c>
+      <c r="E255" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B256" s="1">
+        <v>8.2</v>
+      </c>
+      <c r="C256" s="1">
+        <v>5</v>
+      </c>
+      <c r="D256" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="E256" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated - Admin Edit and Delete functions
</commit_message>
<xml_diff>
--- a/view/site/new.xlsx
+++ b/view/site/new.xlsx
@@ -419,7 +419,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F171"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3824,6 +3824,306 @@
         <v>11</v>
       </c>
       <c r="F171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" t="s">
+        <v>0</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172">
+        <v>8</v>
+      </c>
+      <c r="D172">
+        <v>5</v>
+      </c>
+      <c r="E172">
+        <v>8</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" t="s">
+        <v>2</v>
+      </c>
+      <c r="B173" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173">
+        <v>8.3</v>
+      </c>
+      <c r="D173">
+        <v>5</v>
+      </c>
+      <c r="E173">
+        <v>7.3</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" t="s">
+        <v>4</v>
+      </c>
+      <c r="B174" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174">
+        <v>8.4</v>
+      </c>
+      <c r="D174">
+        <v>5</v>
+      </c>
+      <c r="E174">
+        <v>7.2</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" t="s">
+        <v>6</v>
+      </c>
+      <c r="B175" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175">
+        <v>8.1</v>
+      </c>
+      <c r="D175">
+        <v>5</v>
+      </c>
+      <c r="E175">
+        <v>7.5</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" t="s">
+        <v>8</v>
+      </c>
+      <c r="B176" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176">
+        <v>8</v>
+      </c>
+      <c r="D176">
+        <v>5</v>
+      </c>
+      <c r="E176">
+        <v>8</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" t="s">
+        <v>10</v>
+      </c>
+      <c r="B177" t="s">
+        <v>11</v>
+      </c>
+      <c r="C177">
+        <v>8.2</v>
+      </c>
+      <c r="D177">
+        <v>5</v>
+      </c>
+      <c r="E177">
+        <v>7.4</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" t="s">
+        <v>12</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>8</v>
+      </c>
+      <c r="D178">
+        <v>5</v>
+      </c>
+      <c r="E178">
+        <v>8</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" t="s">
+        <v>13</v>
+      </c>
+      <c r="B179" t="s">
+        <v>3</v>
+      </c>
+      <c r="C179">
+        <v>8.3</v>
+      </c>
+      <c r="D179">
+        <v>5</v>
+      </c>
+      <c r="E179">
+        <v>7.3</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" t="s">
+        <v>14</v>
+      </c>
+      <c r="B180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180">
+        <v>8.4</v>
+      </c>
+      <c r="D180">
+        <v>5</v>
+      </c>
+      <c r="E180">
+        <v>7.2</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" t="s">
+        <v>15</v>
+      </c>
+      <c r="B181" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181">
+        <v>8.1</v>
+      </c>
+      <c r="D181">
+        <v>5</v>
+      </c>
+      <c r="E181">
+        <v>7.5</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" t="s">
+        <v>16</v>
+      </c>
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>8</v>
+      </c>
+      <c r="D182">
+        <v>5</v>
+      </c>
+      <c r="E182">
+        <v>8</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" t="s">
+        <v>17</v>
+      </c>
+      <c r="B183" t="s">
+        <v>11</v>
+      </c>
+      <c r="C183">
+        <v>8.2</v>
+      </c>
+      <c r="D183">
+        <v>5</v>
+      </c>
+      <c r="E183">
+        <v>7.4</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" t="s">
+        <v>18</v>
+      </c>
+      <c r="C184">
+        <v>8</v>
+      </c>
+      <c r="D184">
+        <v>5</v>
+      </c>
+      <c r="E184">
+        <v>8</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" t="s">
+        <v>19</v>
+      </c>
+      <c r="B185" t="s">
+        <v>20</v>
+      </c>
+      <c r="C185">
+        <v>8.1</v>
+      </c>
+      <c r="D185">
+        <v>5</v>
+      </c>
+      <c r="E185">
+        <v>10</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" t="s">
+        <v>2</v>
+      </c>
+      <c r="B186" t="s">
+        <v>20</v>
+      </c>
+      <c r="C186">
+        <v>8.15</v>
+      </c>
+      <c r="D186">
+        <v>5.1</v>
+      </c>
+      <c r="E186">
+        <v>11</v>
+      </c>
+      <c r="F186">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Holidays add to calendar - Done
</commit_message>
<xml_diff>
--- a/view/site/new.xlsx
+++ b/view/site/new.xlsx
@@ -413,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A101" sqref="A101"/>
@@ -2998,6 +2998,406 @@
         <v>7.4</v>
       </c>
       <c r="F130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>8</v>
+      </c>
+      <c r="D131">
+        <v>5</v>
+      </c>
+      <c r="E131">
+        <v>8</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" t="s">
+        <v>3</v>
+      </c>
+      <c r="C132">
+        <v>8.3</v>
+      </c>
+      <c r="D132">
+        <v>5</v>
+      </c>
+      <c r="E132">
+        <v>7.3</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133">
+        <v>8.4</v>
+      </c>
+      <c r="D133">
+        <v>5</v>
+      </c>
+      <c r="E133">
+        <v>7.2</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134">
+        <v>8.1</v>
+      </c>
+      <c r="D134">
+        <v>5</v>
+      </c>
+      <c r="E134">
+        <v>7.5</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135">
+        <v>8</v>
+      </c>
+      <c r="D135">
+        <v>5</v>
+      </c>
+      <c r="E135">
+        <v>8</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136" t="s">
+        <v>11</v>
+      </c>
+      <c r="C136">
+        <v>8.2</v>
+      </c>
+      <c r="D136">
+        <v>5</v>
+      </c>
+      <c r="E136">
+        <v>7.4</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
+        <v>14</v>
+      </c>
+      <c r="B137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137">
+        <v>8.4</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+      <c r="E137">
+        <v>7.2</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" t="s">
+        <v>15</v>
+      </c>
+      <c r="B138" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>8.1</v>
+      </c>
+      <c r="D138">
+        <v>5</v>
+      </c>
+      <c r="E138">
+        <v>7.5</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
+        <v>16</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139">
+        <v>8</v>
+      </c>
+      <c r="D139">
+        <v>5</v>
+      </c>
+      <c r="E139">
+        <v>8</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>17</v>
+      </c>
+      <c r="B140" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140">
+        <v>8.2</v>
+      </c>
+      <c r="D140">
+        <v>5</v>
+      </c>
+      <c r="E140">
+        <v>7.4</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>8</v>
+      </c>
+      <c r="D141">
+        <v>5</v>
+      </c>
+      <c r="E141">
+        <v>8</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
+        <v>2</v>
+      </c>
+      <c r="B142" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142">
+        <v>8.3</v>
+      </c>
+      <c r="D142">
+        <v>5</v>
+      </c>
+      <c r="E142">
+        <v>7.3</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <v>8.4</v>
+      </c>
+      <c r="D143">
+        <v>5</v>
+      </c>
+      <c r="E143">
+        <v>7.2</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144">
+        <v>8.1</v>
+      </c>
+      <c r="D144">
+        <v>5</v>
+      </c>
+      <c r="E144">
+        <v>7.5</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145">
+        <v>8</v>
+      </c>
+      <c r="D145">
+        <v>5</v>
+      </c>
+      <c r="E145">
+        <v>8</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>10</v>
+      </c>
+      <c r="B146" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146">
+        <v>8.2</v>
+      </c>
+      <c r="D146">
+        <v>5</v>
+      </c>
+      <c r="E146">
+        <v>7.4</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>14</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147">
+        <v>8.4</v>
+      </c>
+      <c r="D147">
+        <v>5</v>
+      </c>
+      <c r="E147">
+        <v>7.2</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
+        <v>15</v>
+      </c>
+      <c r="B148" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148">
+        <v>8.1</v>
+      </c>
+      <c r="D148">
+        <v>5</v>
+      </c>
+      <c r="E148">
+        <v>7.5</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
+        <v>16</v>
+      </c>
+      <c r="B149" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149">
+        <v>8</v>
+      </c>
+      <c r="D149">
+        <v>5</v>
+      </c>
+      <c r="E149">
+        <v>8</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>17</v>
+      </c>
+      <c r="B150" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150">
+        <v>8.2</v>
+      </c>
+      <c r="D150">
+        <v>5</v>
+      </c>
+      <c r="E150">
+        <v>7.4</v>
+      </c>
+      <c r="F150">
         <v>0</v>
       </c>
     </row>

</xml_diff>